<commit_message>
test additives in gravure printing
</commit_message>
<xml_diff>
--- a/tests/data/gravure_printing_test.xlsx
+++ b/tests/data/gravure_printing_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -130,6 +130,12 @@
     <t xml:space="preserve">Solute 1 Concentration [mM]</t>
   </si>
   <si>
+    <t xml:space="preserve">Additive 1 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additive 1 Concentration [mg/ml]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coating Speed [m/min]</t>
   </si>
   <si>
@@ -215,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">PbI2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starch</t>
   </si>
   <si>
     <t xml:space="preserve">R2R</t>
@@ -326,24 +335,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -599,421 +612,435 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2:AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="36" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="47" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AH2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AI2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AT2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AU2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AV2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="5" t="s">
         <v>49</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="0" t="str">
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="str">
         <f aca="false">CONCATENATE("SAU_",B3,"_",C3,"_",D3,"_C-",E3)</f>
         <v>SAU_GeSo_1_1_C-1</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="G3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="L3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="0" t="n">
+      <c r="L3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="T3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="S3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AR3" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT3" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU3" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AX3" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="W3" s="0" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="X3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="AD3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AG3" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI3" s="0" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="AJ3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="AL3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN3" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="AP3" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="AQ3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AT3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU3" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="AW3" s="0" t="n">
+      <c r="AY3" s="1" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:R1"/>
-    <mergeCell ref="S1:AW1"/>
+    <mergeCell ref="S1:AY1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>